<commit_message>
novos graficos e fixes
</commit_message>
<xml_diff>
--- a/dados/redessociais.xlsx
+++ b/dados/redessociais.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Grupo-5\dados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Folha 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Rede Social</t>
   </si>
@@ -47,24 +54,16 @@
     <t>Pinterest</t>
   </si>
   <si>
-    <t>Outro</t>
+    <t>Outras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1">
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -102,21 +101,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -127,23 +126,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -342,7 +403,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -361,7 +422,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -391,7 +452,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -417,7 +478,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -443,7 +504,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -469,7 +530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -495,7 +556,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -521,7 +582,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -547,7 +608,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -573,7 +634,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -599,7 +660,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -612,9 +673,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -631,7 +698,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -650,7 +717,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -676,7 +743,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -702,7 +769,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -728,7 +795,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -754,7 +821,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -780,7 +847,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -806,7 +873,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -832,7 +899,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -858,7 +925,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -884,7 +951,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -897,9 +964,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -913,7 +986,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -932,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -962,7 +1035,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -988,7 +1061,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1014,7 +1087,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1040,7 +1113,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1066,7 +1139,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1092,7 +1165,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1118,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1144,7 +1217,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1170,7 +1243,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1183,113 +1256,121 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="1" customWidth="1"/>
-    <col min="3" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.05" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="20.05" customHeight="1">
-      <c r="A2" t="s" s="2">
+    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="2">
+    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="2">
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>68</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="2">
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="2">
+    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="2">
+    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>55</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="2">
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="2">
+    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="2">
+    <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="2">
+    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="3">
@@ -1297,8 +1378,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>